<commit_message>
WIP. Several things broke. Sad day
</commit_message>
<xml_diff>
--- a/Output/Tracked_expenses.xlsx
+++ b/Output/Tracked_expenses.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -37,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -51,15 +54,44 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,9 +466,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>Month</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -459,56 +496,24 @@
           <t>Recreational</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 5</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 6</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 7</t>
-        </is>
-      </c>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Subscriptions</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 9</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 10</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 11</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 12</t>
-        </is>
-      </c>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Unaccounted</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 14</t>
-        </is>
-      </c>
+      <c r="P1" s="1" t="n"/>
       <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Total Sum</t>
@@ -519,264 +524,833 @@
           <t>Balance</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>('Savings', '/')</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>('Eating Out Work', '/')</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>('Uber To Work', '/')</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>('Recreational', 'Uber Eats')</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>('Recreational', 'Bars And Restaurants')</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>('Recreational', 'Bizum')</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>('Recreational', 'Bazar')</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>('Subscriptions', 'Psychologist')</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>('Subscriptions', 'Dystopia')</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>('Subscriptions', 'ChatGPT')</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>('Subscriptions', 'Gym')</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>('Subscriptions', 'Public Transport')</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>('Unaccounted', 'Withdrawals')</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>('Unaccounted', 'Unknown')</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>('Total Sum', '/')</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>('Balance', '/')</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Subcategory</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Uber Eats</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>Bars And Restaurants</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>Bizum</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>Bazar</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>Psychologist</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>Dystopia</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>ChatGPT</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>Gym</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>Public Transport</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>Withdrawals</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>Unknown</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-33.3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-33.93</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-446.12</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-135.4</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-201</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-15</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-140</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-429.7000000000004</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-914.65</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-1344.35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
+      <c r="B5" s="2" t="n">
+        <v>45047</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-15</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-71.88</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-611.9600000000002</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-125.74</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-131.55</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-76.8</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-230</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-443.4999999999998</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1067.83</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-1511.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45078</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-15</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-166.23</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-241.41</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1032.96</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-71.20999999999999</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-210</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-15</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-28.8</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-150</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-50.53999999999905</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1815.51</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-1866.049999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45108</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-44.90000000000001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-171.02</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-63.38</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-751.1899999999999</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-263.15</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-206.1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-31.8</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>87.39999999999895</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-1566.44</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-1479.040000000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>45139</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-124.95</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-252.1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-136.77</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-609.48</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-216.55</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-113.64</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-31.8</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-200</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-586.73</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-1520.19</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-2106.92</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-88.65000000000001</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-585.8100000000001</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-83.19</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-374.77</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-220.03</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-170.03</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-15</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-34.8</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-350</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-142.7999999999995</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-1607.18</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-1749.98</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>45200</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-120.6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-322.3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-34.82</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-406.8699999999999</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-67</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-163.64</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-31.8</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-130</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-265.6500000000017</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-1181.93</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-1447.580000000002</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>45231</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-85.94999999999999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-166.61</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-96.56</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-351.2</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-732.2600000000001</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-131.42</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-15</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-43.55</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>151.1800000000007</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-1657.45</v>
+      </c>
+      <c r="R11" t="n">
+        <v>-1506.27</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>45261</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-48.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-148.73</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-166.14</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-479.21</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-314.78</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-139.32</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-210</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-23.18</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-3</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-115.8000000000002</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-1567.76</v>
+      </c>
+      <c r="R12" t="n">
+        <v>-1683.56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>45292</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-64.25</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-213.9</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-292.18</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-204.82</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-86.5</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-15</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-22.92</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-34.9</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-280</v>
+      </c>
+      <c r="P13" t="n">
+        <v>-639.51</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-934.47</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-1573.98</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>45323</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-86.79999999999998</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-228.61</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-78.65000000000001</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-377.8700000000001</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-85.62</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-349.23</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>-23.21</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-37.9</v>
+      </c>
+      <c r="N14" t="n">
+        <v>-33.17</v>
+      </c>
+      <c r="O14" t="n">
+        <v>-280</v>
+      </c>
+      <c r="P14" t="n">
+        <v>-294.1699999999996</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-1301.06</v>
+      </c>
+      <c r="R14" t="n">
+        <v>-1595.23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>45352</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-69.7</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-121.71</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-101.23</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-428.47</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-159.4</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-86.23000000000002</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-15</v>
+      </c>
+      <c r="L15" t="n">
+        <v>-22.94</v>
+      </c>
+      <c r="M15" t="n">
+        <v>-37.9</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-140</v>
+      </c>
+      <c r="P15" t="n">
+        <v>16.07000000000039</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>-1042.58</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-1026.51</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>45383</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
         <v>-29.25</v>
       </c>
-      <c r="U3" t="n">
+      <c r="E16" t="n">
         <v>-72.12</v>
       </c>
-      <c r="V3" t="n">
+      <c r="F16" t="n">
         <v>-79.5</v>
       </c>
-      <c r="W3" t="n">
+      <c r="G16" t="n">
         <v>-195.83</v>
       </c>
-      <c r="X3" t="n">
+      <c r="H16" t="n">
         <v>-81.25</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="I16" t="n">
         <v>-53.69</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="J16" t="n">
         <v>-210</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="K16" t="n">
         <v>-15</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="L16" t="n">
         <v>-23.1</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="M16" t="n">
         <v>-37.9</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="N16" t="n">
         <v>-28.8</v>
       </c>
-      <c r="AE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="n">
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
         <v>-145.4500000000004</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="Q16" t="n">
         <v>-826.4399999999999</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="R16" t="n">
         <v>-971.8900000000003</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>